<commit_message>
Fixed a minor syntax problem with the examples for verbatimCoordinateSystem so that the conversion to RDF works.
</commit_message>
<xml_diff>
--- a/HISPID2015.xlsx
+++ b/HISPID2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="HISPID2015" sheetId="1" r:id="rId1"/>
@@ -1868,9 +1868,6 @@
     <t>This may not reflect the currently political boundaries</t>
   </si>
   <si>
-    <t>"decimal degrees", "UTM"; "NZMG"</t>
-  </si>
-  <si>
     <t>spadat</t>
   </si>
   <si>
@@ -2304,6 +2301,9 @@
   </si>
   <si>
     <t>ac:furtherInformationURL</t>
+  </si>
+  <si>
+    <t>"decimal degrees", "UTM", "NZMG"</t>
   </si>
 </sst>
 </file>
@@ -3001,7 +3001,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3036,7 +3036,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3213,7 +3213,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3224,34 +3224,34 @@
   <dimension ref="A1:R260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="50.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="42.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="67.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="65.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="87.85546875" style="2" customWidth="1"/>
-    <col min="15" max="16" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="50.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="42.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="67.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="65.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="87.88671875" style="2" customWidth="1"/>
+    <col min="15" max="16" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="53" style="2" customWidth="1"/>
-    <col min="18" max="18" width="49.5703125" customWidth="1"/>
+    <col min="18" max="18" width="49.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3304,10 +3304,10 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -3427,10 +3427,10 @@
         <v>30</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -3511,10 +3511,10 @@
         <v>36</v>
       </c>
       <c r="R6" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -3557,10 +3557,10 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="6" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -3576,22 +3576,22 @@
         <v>http://purl.org/dc/terms/rightsHolder</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>267</v>
       </c>
       <c r="R8" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>568</v>
@@ -3622,10 +3622,10 @@
         <v>267</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3838,10 +3838,10 @@
         <v>57</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>40</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
@@ -4026,7 +4026,7 @@
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
     </row>
-    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -4142,10 +4142,10 @@
         <v>508</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -4175,10 +4175,10 @@
         <v>519</v>
       </c>
       <c r="R22" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="15" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="15" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>40</v>
       </c>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="Q24" s="12"/>
     </row>
-    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/33</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/15</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>94</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>94</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>94</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>94</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>94</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>94</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>94</v>
       </c>
@@ -4725,10 +4725,10 @@
         <v>465</v>
       </c>
       <c r="R36" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>94</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>129</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>129</v>
       </c>
@@ -4842,10 +4842,10 @@
         <v>133</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>129</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>129</v>
       </c>
@@ -4922,10 +4922,10 @@
         <v>145</v>
       </c>
       <c r="R41" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>129</v>
       </c>
@@ -4968,10 +4968,10 @@
         <v>151</v>
       </c>
       <c r="R42" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>129</v>
       </c>
@@ -5014,10 +5014,10 @@
         <v>466</v>
       </c>
       <c r="R43" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>129</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>129</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>129</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>129</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>129</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>129</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>129</v>
       </c>
@@ -5276,10 +5276,10 @@
         <v>187</v>
       </c>
       <c r="P50" s="12" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>129</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>129</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>129</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>129</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/verbatim_coordinate_system.xml</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>616</v>
+        <v>761</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>505</v>
@@ -5443,7 +5443,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>129</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>129</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>129</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>129</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>129</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>129</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>129</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>129</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>129</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>129</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>129</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>129</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>129</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>129</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>129</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>129</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>129</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>268</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>268</v>
       </c>
@@ -6134,10 +6134,10 @@
         <v>275</v>
       </c>
       <c r="R73" s="6" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>268</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>268</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>268</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>268</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>268</v>
       </c>
@@ -6329,10 +6329,10 @@
         <v>290</v>
       </c>
       <c r="R78" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>268</v>
       </c>
@@ -6369,10 +6369,10 @@
         <v>293</v>
       </c>
       <c r="R79" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>268</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>268</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>268</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>268</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>268</v>
       </c>
@@ -6556,7 +6556,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>268</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>268</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>319</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>319</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>319</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>319</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>319</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>319</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>319</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>319</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>319</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>319</v>
       </c>
@@ -7001,10 +7001,10 @@
         <v>355</v>
       </c>
       <c r="R96" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>319</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>319</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>319</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>319</v>
       </c>
@@ -7149,10 +7149,10 @@
         <v>367</v>
       </c>
       <c r="R100" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>319</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>319</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>319</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>319</v>
       </c>
@@ -7301,7 +7301,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>319</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/11</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>319</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>380</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>380</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>380</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>380</v>
       </c>
@@ -7478,12 +7478,12 @@
         <v>598</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>380</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C111" s="3" t="str">
         <f t="shared" si="8"/>
@@ -7516,7 +7516,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>380</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>380</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>393</v>
       </c>
@@ -7625,7 +7625,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>393</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>393</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>393</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>393</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>393</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>393</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>418</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>418</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>418</v>
       </c>
@@ -7920,7 +7920,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>418</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="125" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>418</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>418</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>418</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>418</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>418</v>
       </c>
@@ -8101,7 +8101,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>418</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>https://github.com/hiscom/hispid-review-2014-15/issues/10</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>581</v>
       </c>
@@ -8153,10 +8153,10 @@
         <v>267</v>
       </c>
       <c r="R131" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>581</v>
       </c>
@@ -8182,10 +8182,10 @@
         <v>267</v>
       </c>
       <c r="R132" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>581</v>
       </c>
@@ -8211,10 +8211,10 @@
         <v>267</v>
       </c>
       <c r="R133" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>581</v>
       </c>
@@ -8240,10 +8240,10 @@
         <v>267</v>
       </c>
       <c r="R134" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>581</v>
       </c>
@@ -8266,10 +8266,10 @@
         <v>267</v>
       </c>
       <c r="R135" s="10" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>581</v>
       </c>
@@ -8292,10 +8292,10 @@
         <v>267</v>
       </c>
       <c r="R136" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>581</v>
       </c>
@@ -8318,10 +8318,10 @@
         <v>267</v>
       </c>
       <c r="R137" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>581</v>
       </c>
@@ -8347,10 +8347,10 @@
         <v>267</v>
       </c>
       <c r="R138" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>581</v>
       </c>
@@ -8379,10 +8379,10 @@
         <v>591</v>
       </c>
       <c r="R139" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>581</v>
       </c>
@@ -8405,10 +8405,10 @@
         <v>267</v>
       </c>
       <c r="R140" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>581</v>
       </c>
@@ -8431,10 +8431,10 @@
         <v>267</v>
       </c>
       <c r="R141" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>581</v>
       </c>
@@ -8457,10 +8457,10 @@
         <v>267</v>
       </c>
       <c r="R142" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>581</v>
       </c>
@@ -8483,10 +8483,10 @@
         <v>267</v>
       </c>
       <c r="R143" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>581</v>
       </c>
@@ -8509,10 +8509,10 @@
         <v>267</v>
       </c>
       <c r="R144" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>581</v>
       </c>
@@ -8535,24 +8535,24 @@
         <v>267</v>
       </c>
       <c r="R145" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C146" s="17" t="s">
         <v>549</v>
       </c>
       <c r="D146" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="E146" t="s">
         <v>622</v>
-      </c>
-      <c r="E146" t="s">
-        <v>623</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>20</v>
@@ -8561,56 +8561,56 @@
         <v>267</v>
       </c>
       <c r="R146" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D147" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="E147" t="s">
         <v>628</v>
       </c>
-      <c r="E147" t="s">
+      <c r="F147" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G147" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="F147" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G147" s="2" t="s">
+      <c r="H147" t="s">
         <v>630</v>
-      </c>
-      <c r="H147" t="s">
-        <v>631</v>
       </c>
       <c r="K147" s="2" t="s">
         <v>267</v>
       </c>
       <c r="R147" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C148" s="17" t="s">
         <v>545</v>
       </c>
       <c r="D148" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E148" t="s">
         <v>633</v>
-      </c>
-      <c r="E148" t="s">
-        <v>634</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>28</v>
@@ -8622,24 +8622,24 @@
         <v>267</v>
       </c>
       <c r="R148" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D149" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="E149" s="10" t="s">
         <v>638</v>
-      </c>
-      <c r="E149" s="10" t="s">
-        <v>639</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>20</v>
@@ -8648,24 +8648,24 @@
         <v>267</v>
       </c>
       <c r="R149" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C150" s="17" t="s">
         <v>549</v>
       </c>
       <c r="D150" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="E150" t="s">
         <v>642</v>
-      </c>
-      <c r="E150" t="s">
-        <v>643</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>28</v>
@@ -8677,24 +8677,24 @@
         <v>267</v>
       </c>
       <c r="R150" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D151" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="E151" t="s">
         <v>646</v>
-      </c>
-      <c r="E151" t="s">
-        <v>647</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>20</v>
@@ -8703,53 +8703,53 @@
         <v>267</v>
       </c>
       <c r="R151" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="152" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>549</v>
       </c>
       <c r="D152" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="E152" s="6" t="s">
         <v>650</v>
       </c>
-      <c r="E152" s="6" t="s">
+      <c r="F152" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I152" s="2" t="s">
         <v>651</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I152" s="2" t="s">
-        <v>652</v>
       </c>
       <c r="K152" s="2" t="s">
         <v>267</v>
       </c>
       <c r="R152" s="6" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>545</v>
       </c>
       <c r="D153" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E153" t="s">
         <v>680</v>
-      </c>
-      <c r="E153" t="s">
-        <v>681</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>20</v>
@@ -8758,24 +8758,24 @@
         <v>267</v>
       </c>
       <c r="R153" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>545</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E154" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>20</v>
@@ -8784,24 +8784,24 @@
         <v>267</v>
       </c>
       <c r="R154" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E155" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>20</v>
@@ -8810,24 +8810,24 @@
         <v>267</v>
       </c>
       <c r="R155" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E156" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>20</v>
@@ -8836,24 +8836,24 @@
         <v>267</v>
       </c>
       <c r="R156" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D157" s="17" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E157" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>20</v>
@@ -8862,24 +8862,24 @@
         <v>267</v>
       </c>
       <c r="R157" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="158" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C158" s="19" t="s">
         <v>520</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>20</v>
@@ -8888,24 +8888,24 @@
         <v>267</v>
       </c>
       <c r="R158" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>20</v>
@@ -8914,24 +8914,24 @@
         <v>267</v>
       </c>
       <c r="R159" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C160" s="17" t="s">
         <v>520</v>
       </c>
       <c r="D160" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="E160" t="s">
         <v>691</v>
-      </c>
-      <c r="E160" t="s">
-        <v>692</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>20</v>
@@ -8940,24 +8940,24 @@
         <v>267</v>
       </c>
       <c r="R160" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D161" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="E161" s="2" t="s">
         <v>699</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>700</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>20</v>
@@ -8966,24 +8966,24 @@
         <v>267</v>
       </c>
       <c r="R161" s="20" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D162" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="E162" t="s">
         <v>710</v>
-      </c>
-      <c r="E162" t="s">
-        <v>711</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>20</v>
@@ -8992,24 +8992,24 @@
         <v>267</v>
       </c>
       <c r="R162" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C163" s="17" t="s">
         <v>509</v>
       </c>
       <c r="D163" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="E163" t="s">
         <v>718</v>
-      </c>
-      <c r="E163" t="s">
-        <v>719</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>20</v>
@@ -9018,21 +9018,21 @@
         <v>267</v>
       </c>
       <c r="R163" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B164" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C164" s="17" t="s">
         <v>520</v>
       </c>
       <c r="D164" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="E164" t="s">
         <v>732</v>
-      </c>
-      <c r="E164" t="s">
-        <v>733</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>20</v>
@@ -9041,53 +9041,53 @@
         <v>267</v>
       </c>
       <c r="R164" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="165" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D165" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="E165" t="s">
         <v>736</v>
       </c>
-      <c r="E165" t="s">
+      <c r="F165" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G165" s="2" t="s">
         <v>737</v>
-      </c>
-      <c r="F165" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G165" s="2" t="s">
-        <v>738</v>
       </c>
       <c r="K165" s="2" t="s">
         <v>267</v>
       </c>
       <c r="R165" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>581</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E166" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>20</v>
@@ -9096,24 +9096,24 @@
         <v>267</v>
       </c>
       <c r="R166" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A167" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="B167" s="4" t="s">
         <v>743</v>
-      </c>
-    </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>744</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D167" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="E167" t="s">
         <v>745</v>
-      </c>
-      <c r="E167" t="s">
-        <v>746</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>20</v>
@@ -9122,56 +9122,56 @@
         <v>267</v>
       </c>
       <c r="R167" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="B168" s="4" t="s">
         <v>747</v>
-      </c>
-    </row>
-    <row r="168" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>748</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>543</v>
       </c>
       <c r="D168" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="E168" t="s">
+        <v>748</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H168" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="E168" t="s">
-        <v>749</v>
-      </c>
-      <c r="F168" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H168" s="2" t="s">
+      <c r="I168" s="2" t="s">
         <v>751</v>
-      </c>
-      <c r="I168" s="2" t="s">
-        <v>752</v>
       </c>
       <c r="K168" s="2" t="s">
         <v>267</v>
       </c>
       <c r="R168" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D169" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="E169" t="s">
         <v>755</v>
-      </c>
-      <c r="E169" t="s">
-        <v>756</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>20</v>
@@ -9180,24 +9180,24 @@
         <v>267</v>
       </c>
       <c r="R169" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A170" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="B170" s="4" t="s">
         <v>757</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>758</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>520</v>
       </c>
       <c r="D170" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="E170" t="s">
         <v>759</v>
-      </c>
-      <c r="E170" t="s">
-        <v>760</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>20</v>
@@ -9206,277 +9206,277 @@
         <v>267</v>
       </c>
       <c r="R170" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B171" s="18"/>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B172" s="18"/>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B173" s="18"/>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B174" s="18"/>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B175" s="18"/>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B176" s="18"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="18"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="18"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="18"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="18"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="18"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="18"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="18"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="18"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="18"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="18"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="18"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="18"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="18"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="18"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="18"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="18"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" s="18"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" s="18"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" s="18"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" s="18"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" s="18"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" s="18"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" s="18"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" s="18"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" s="18"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B202" s="18"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B203" s="18"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B204" s="18"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B205" s="18"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B206" s="18"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B207" s="18"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B208" s="18"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" s="18"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" s="18"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" s="18"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B212" s="18"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B213" s="18"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B214" s="18"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" s="18"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" s="18"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" s="18"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" s="18"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" s="18"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B220" s="18"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B221" s="18"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" s="18"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" s="18"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" s="18"/>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B225" s="18"/>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B226" s="18"/>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B227" s="18"/>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B228" s="18"/>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B229" s="18"/>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B230" s="18"/>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B231" s="18"/>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B232" s="18"/>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B233" s="18"/>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B234" s="18"/>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B235" s="18"/>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B236" s="18"/>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B237" s="18"/>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" s="18"/>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B239" s="18"/>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B240" s="18"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" s="18"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" s="18"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" s="18"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" s="18"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" s="18"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" s="18"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" s="18"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" s="18"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" s="18"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" s="18"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" s="18"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" s="18"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" s="18"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B254" s="18"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B255" s="18"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" s="18"/>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B257" s="18"/>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B258" s="18"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B259" s="18"/>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B260" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes to HISPID2015.xlsx
</commit_message>
<xml_diff>
--- a/HISPID2015.xlsx
+++ b/HISPID2015.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="760">
   <si>
     <t>group</t>
   </si>
@@ -2161,9 +2161,6 @@
     <t>dwc:vernacularName</t>
   </si>
   <si>
-    <t>scientificNameId</t>
-  </si>
-  <si>
     <t>dwc:scientificNameID</t>
   </si>
   <si>
@@ -2275,9 +2272,6 @@
     <t>variant</t>
   </si>
   <si>
-    <t>MediaItem (Access)</t>
-  </si>
-  <si>
     <t>http://rs.tdwg.org/ac/terms/variant</t>
   </si>
   <si>
@@ -2306,6 +2300,9 @@
   </si>
   <si>
     <t>https://github.com/hiscom/hispid/issues/5</t>
+  </si>
+  <si>
+    <t>scientificNameID</t>
   </si>
 </sst>
 </file>
@@ -3209,10 +3206,10 @@
   <dimension ref="A1:R260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I152" sqref="I152"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,7 +3891,7 @@
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -4229,7 +4226,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -4269,7 +4266,7 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -5723,7 +5720,7 @@
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>505</v>
@@ -6795,7 +6792,7 @@
       </c>
       <c r="Q78" s="4"/>
       <c r="R78" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -6841,7 +6838,7 @@
       </c>
       <c r="Q79" s="4"/>
       <c r="R79" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -7163,7 +7160,7 @@
         <v>320</v>
       </c>
       <c r="C87" s="7" t="str">
-        <f t="shared" ref="C87:C100" si="3">HYPERLINK("http://rs.tdwg.org/dwc/terms")</f>
+        <f t="shared" ref="C87:C101" si="3">HYPERLINK("http://rs.tdwg.org/dwc/terms")</f>
         <v>http://rs.tdwg.org/dwc/terms</v>
       </c>
       <c r="D87" s="7" t="str">
@@ -7547,23 +7544,21 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C96" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>http://rs.tdwg.org/dwc/terms</v>
-      </c>
-      <c r="D96" s="7" t="str">
-        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/scientificName")</f>
-        <v>http://rs.tdwg.org/dwc/terms/scientificName</v>
+        <v>759</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>713</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>353</v>
+        <v>714</v>
       </c>
       <c r="F96" s="4" t="s">
         <v>20</v>
@@ -7571,267 +7566,263 @@
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
-      <c r="J96" s="4" t="s">
-        <v>354</v>
-      </c>
+      <c r="J96" s="4"/>
       <c r="K96" s="4" t="s">
-        <v>22</v>
+        <v>267</v>
       </c>
       <c r="L96" s="4"/>
       <c r="M96" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="N96" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="O96" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="P96" s="4" t="s">
-        <v>355</v>
-      </c>
+        <v>759</v>
+      </c>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
       <c r="Q96" s="4"/>
       <c r="R96" s="4" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C97" s="7" t="str">
         <f t="shared" si="3"/>
         <v>http://rs.tdwg.org/dwc/terms</v>
       </c>
       <c r="D97" s="7" t="str">
-        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/scientificNameAuthorship")</f>
-        <v>http://rs.tdwg.org/dwc/terms/scientificNameAuthorship</v>
+        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/scientificName")</f>
+        <v>http://rs.tdwg.org/dwc/terms/scientificName</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
-      <c r="I97" s="4" t="s">
-        <v>489</v>
-      </c>
+      <c r="I97" s="4"/>
       <c r="J97" s="4" t="s">
-        <v>490</v>
+        <v>354</v>
       </c>
       <c r="K97" s="4" t="s">
         <v>22</v>
       </c>
       <c r="L97" s="4"/>
       <c r="M97" s="4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="N97" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O97" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="P97" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Q97" s="4"/>
-      <c r="R97" s="4"/>
-    </row>
-    <row r="98" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="R97" s="4" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C98" s="7" t="str">
         <f t="shared" si="3"/>
         <v>http://rs.tdwg.org/dwc/terms</v>
       </c>
       <c r="D98" s="7" t="str">
-        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/nomenclaturalCode")</f>
-        <v>http://rs.tdwg.org/dwc/terms/nomenclaturalCode</v>
+        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/scientificNameAuthorship")</f>
+        <v>http://rs.tdwg.org/dwc/terms/scientificNameAuthorship</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G98" s="4"/>
-      <c r="H98" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="I98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4" t="s">
+        <v>489</v>
+      </c>
       <c r="J98" s="4" t="s">
-        <v>362</v>
+        <v>490</v>
       </c>
       <c r="K98" s="4" t="s">
-        <v>505</v>
+        <v>22</v>
       </c>
       <c r="L98" s="4"/>
       <c r="M98" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="N98" s="4"/>
-      <c r="O98" s="4"/>
-      <c r="P98" s="4"/>
+        <v>356</v>
+      </c>
+      <c r="N98" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="P98" s="4" t="s">
+        <v>358</v>
+      </c>
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C99" s="7" t="str">
         <f t="shared" si="3"/>
         <v>http://rs.tdwg.org/dwc/terms</v>
       </c>
       <c r="D99" s="7" t="str">
-        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/taxonRemarks")</f>
-        <v>http://rs.tdwg.org/dwc/terms/taxonRemarks</v>
-      </c>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
+        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/nomenclaturalCode")</f>
+        <v>http://rs.tdwg.org/dwc/terms/nomenclaturalCode</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
+      <c r="H99" s="7" t="s">
+        <v>361</v>
+      </c>
       <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
+      <c r="J99" s="4" t="s">
+        <v>362</v>
+      </c>
       <c r="K99" s="4" t="s">
-        <v>267</v>
+        <v>505</v>
       </c>
       <c r="L99" s="4"/>
       <c r="M99" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="N99" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="O99" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="P99" s="4" t="s">
-        <v>364</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C100" s="7" t="str">
         <f t="shared" si="3"/>
         <v>http://rs.tdwg.org/dwc/terms</v>
       </c>
       <c r="D100" s="7" t="str">
+        <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/taxonRemarks")</f>
+        <v>http://rs.tdwg.org/dwc/terms/taxonRemarks</v>
+      </c>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="N100" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="O100" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="P100" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="4"/>
+    </row>
+    <row r="101" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="C101" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>http://rs.tdwg.org/dwc/terms</v>
+      </c>
+      <c r="D101" s="7" t="str">
         <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/vernacularName")</f>
         <v>http://rs.tdwg.org/dwc/terms/vernacularName</v>
       </c>
-      <c r="E100" s="4" t="s">
+      <c r="E101" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="F100" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4" t="s">
+      <c r="F101" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="J100" s="4"/>
-      <c r="K100" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L100" s="4"/>
-      <c r="M100" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="N100" s="4"/>
-      <c r="O100" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="P100" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q100" s="4"/>
-      <c r="R100" s="4" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="C101" s="7" t="str">
-        <f t="shared" ref="C101:C106" si="4">HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms</v>
-      </c>
-      <c r="D101" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/cultivarGroupName")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/cultivarGroupName</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4" t="s">
         <v>22</v>
       </c>
       <c r="L101" s="4"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4" t="s">
-        <v>492</v>
-      </c>
+      <c r="M101" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="N101" s="4"/>
       <c r="O101" s="4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="P101" s="4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="Q101" s="4"/>
-      <c r="R101" s="4"/>
+      <c r="R101" s="4" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="102" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C102" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C102:C107" si="4">HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D102" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/cultivarName")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/cultivarName</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/cultivarGroupName")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/cultivarGroupName</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F102" s="4" t="s">
         <v>20</v>
@@ -7851,10 +7842,10 @@
         <v>492</v>
       </c>
       <c r="O102" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="P102" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
@@ -7864,18 +7855,18 @@
         <v>319</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C103" s="7" t="str">
         <f t="shared" si="4"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D103" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/tradeDesignation")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/tradeDesignation</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/cultivarName")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/cultivarName</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F103" s="4" t="s">
         <v>20</v>
@@ -7892,86 +7883,87 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O103" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="P103" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B104" s="12" t="s">
-        <v>582</v>
+      <c r="B104" s="6" t="s">
+        <v>375</v>
       </c>
       <c r="C104" s="7" t="str">
         <f t="shared" si="4"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D104" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/hybridFlag")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/hybridFlag</v>
-      </c>
-      <c r="E104" s="13" t="s">
-        <v>585</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/tradeDesignation")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/tradeDesignation</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>376</v>
       </c>
       <c r="F104" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G104" s="4"/>
+      <c r="G104" s="4" t="s">
+        <v>370</v>
+      </c>
       <c r="H104" s="4"/>
-      <c r="I104" s="4" t="s">
-        <v>588</v>
-      </c>
+      <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="L104" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/11")</f>
-        <v>https://github.com/hiscom/hispid/issues/11</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L104" s="4"/>
       <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
+      <c r="N104" s="4" t="s">
+        <v>493</v>
+      </c>
       <c r="O104" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P104" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>319</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C105" s="7" t="str">
         <f t="shared" si="4"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D105" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/hybridParent1")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/hybridParent1</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>586</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/hybridFlag")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/hybridFlag</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>585</v>
       </c>
       <c r="F105" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
+      <c r="I105" s="4" t="s">
+        <v>588</v>
+      </c>
       <c r="J105" s="4"/>
       <c r="K105" s="4" t="s">
         <v>267</v>
@@ -7982,8 +7974,12 @@
       </c>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
+      <c r="O105" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="P105" s="4" t="s">
+        <v>378</v>
+      </c>
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
@@ -7992,18 +7988,18 @@
         <v>319</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C106" s="7" t="str">
         <f t="shared" si="4"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D106" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/hybridParent2")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/hybridParent2</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/hybridParent1")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/hybridParent1</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F106" s="4" t="s">
         <v>20</v>
@@ -8021,32 +8017,28 @@
       </c>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
-      <c r="O106" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="P106" s="4" t="s">
-        <v>379</v>
-      </c>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>381</v>
+        <v>319</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>584</v>
       </c>
       <c r="C107" s="7" t="str">
-        <f t="shared" ref="C107:C130" si="5">HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
+        <f t="shared" si="4"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D107" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/miscellaneousRemarks")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/miscellaneousRemarks</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/hybridParent2")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/hybridParent2</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>382</v>
+        <v>587</v>
       </c>
       <c r="F107" s="4" t="s">
         <v>20</v>
@@ -8056,21 +8048,19 @@
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4" t="s">
-        <v>22</v>
+        <v>267</v>
       </c>
       <c r="L107" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/1")</f>
-        <v>https://github.com/hiscom/hispid/issues/1</v>
+        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/11")</f>
+        <v>https://github.com/hiscom/hispid/issues/11</v>
       </c>
       <c r="M107" s="4"/>
-      <c r="N107" s="4" t="s">
-        <v>383</v>
-      </c>
+      <c r="N107" s="4"/>
       <c r="O107" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="P107" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
@@ -8080,34 +8070,43 @@
         <v>380</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>591</v>
+        <v>381</v>
       </c>
       <c r="C108" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
+        <f t="shared" ref="C108:C131" si="5">HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D108" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/exsiccataSeries")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/exsiccataSeries</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/miscellaneousRemarks")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/miscellaneousRemarks</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="F108" s="4"/>
+        <v>382</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="L108" s="7" t="s">
-        <v>759</v>
+        <v>22</v>
+      </c>
+      <c r="L108" s="7" t="str">
+        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/1")</f>
+        <v>https://github.com/hiscom/hispid/issues/1</v>
       </c>
       <c r="M108" s="4"/>
-      <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
+      <c r="N108" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="P108" s="4" t="s">
+        <v>384</v>
+      </c>
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
@@ -8116,18 +8115,18 @@
         <v>380</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C109" s="7" t="str">
         <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D109" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/exsiccataFascicle")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/exsiccataFascicle</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/exsiccataSeries")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/exsiccataSeries</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -8138,7 +8137,7 @@
         <v>505</v>
       </c>
       <c r="L109" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
@@ -8152,18 +8151,18 @@
         <v>380</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C110" s="7" t="str">
         <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D110" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/exsiccataNumber")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/exsiccataNumber</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/exsiccataFascicle")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/exsiccataFascicle</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
@@ -8174,7 +8173,7 @@
         <v>505</v>
       </c>
       <c r="L110" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
@@ -8183,48 +8182,39 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>380</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>615</v>
+        <v>593</v>
       </c>
       <c r="C111" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms")</f>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D111" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/voucherFor")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/voucherFor</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/exsiccataNumber")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/exsiccataNumber</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>596</v>
+      </c>
+      <c r="F111" s="4"/>
       <c r="G111" s="4"/>
-      <c r="H111" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/voucher_for.xml")</f>
-        <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/voucher_for.xml</v>
-      </c>
+      <c r="H111" s="4"/>
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L111" s="4"/>
+        <v>505</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>757</v>
+      </c>
       <c r="M111" s="4"/>
-      <c r="N111" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="O111" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="P111" s="4" t="s">
-        <v>385</v>
-      </c>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
       <c r="Q111" s="4"/>
       <c r="R111" s="4"/>
     </row>
@@ -8233,28 +8223,26 @@
         <v>380</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>386</v>
+        <v>615</v>
       </c>
       <c r="C112" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D112" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/provenanceTypeFlag")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/provenanceTypeFlag</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/voucherFor")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/voucherFor</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>387</v>
+        <v>601</v>
       </c>
       <c r="F112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G112" s="4" t="s">
-        <v>388</v>
-      </c>
+      <c r="G112" s="4"/>
       <c r="H112" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/provenance_type_flag.xml")</f>
-        <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/provenance_type_flag.xml</v>
+        <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/voucher_for.xml")</f>
+        <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/voucher_for.xml</v>
       </c>
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
@@ -8264,44 +8252,45 @@
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
       <c r="N112" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="O112" s="4" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="P112" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="Q112" s="4" t="s">
-        <v>495</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="Q112" s="4"/>
       <c r="R112" s="4"/>
     </row>
-    <row r="113" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>380</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C113" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D113" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/cultivatedPlantProvenance")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/cultivatedPlantProvenance</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/provenanceTypeFlag")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/provenanceTypeFlag</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F113" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="H113" s="4"/>
+        <v>388</v>
+      </c>
+      <c r="H113" s="7" t="str">
+        <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/provenance_type_flag.xml")</f>
+        <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/provenance_type_flag.xml</v>
+      </c>
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4" t="s">
@@ -8309,168 +8298,170 @@
       </c>
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="Q113" s="4"/>
+      <c r="N113" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="O113" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="P113" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q113" s="4" t="s">
+        <v>495</v>
+      </c>
       <c r="R113" s="4"/>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C114" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D114" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/donor")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/donor</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/cultivatedPlantProvenance")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/cultivatedPlantProvenance</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G114" s="4"/>
+      <c r="G114" s="4" t="s">
+        <v>392</v>
+      </c>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4" t="s">
-        <v>267</v>
+        <v>22</v>
       </c>
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
-      <c r="N114" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="O114" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="P114" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q114" s="4" t="s">
-        <v>498</v>
-      </c>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
       <c r="R114" s="4"/>
     </row>
-    <row r="115" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>393</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C115" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D115" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/duplicatesDistributedTo")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/duplicatesDistributedTo</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/donor")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/donor</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G115" s="4" t="s">
-        <v>399</v>
-      </c>
+      <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
-      <c r="J115" s="4" t="s">
-        <v>400</v>
-      </c>
+      <c r="J115" s="4"/>
       <c r="K115" s="4" t="s">
         <v>267</v>
       </c>
       <c r="L115" s="4"/>
       <c r="M115" s="4"/>
       <c r="N115" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="O115" s="4" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="P115" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="Q115" s="4"/>
+        <v>396</v>
+      </c>
+      <c r="Q115" s="4" t="s">
+        <v>498</v>
+      </c>
       <c r="R115" s="4"/>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>393</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C116" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D116" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanIdentifier")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/loanIdentifier</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/duplicatesDistributedTo")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/duplicatesDistributedTo</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F116" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G116" s="4"/>
+      <c r="G116" s="4" t="s">
+        <v>399</v>
+      </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
-      <c r="J116" s="4"/>
+      <c r="J116" s="4" t="s">
+        <v>400</v>
+      </c>
       <c r="K116" s="4" t="s">
-        <v>22</v>
+        <v>267</v>
       </c>
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
       <c r="N116" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="O116" s="4" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="P116" s="4" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="Q116" s="4"/>
       <c r="R116" s="4"/>
     </row>
-    <row r="117" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>393</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C117" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D117" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanDestination")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/loanDestination</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanIdentifier")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/loanIdentifier</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G117" s="4" t="s">
-        <v>407</v>
-      </c>
+      <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
@@ -8480,39 +8471,41 @@
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
       <c r="N117" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O117" s="4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="P117" s="4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="Q117" s="4"/>
       <c r="R117" s="4"/>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>393</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C118" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D118" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanForBotanist")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/loanForBotanist</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanDestination")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/loanDestination</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G118" s="4"/>
+      <c r="G118" s="4" t="s">
+        <v>407</v>
+      </c>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
       <c r="J118" s="4"/>
@@ -8522,13 +8515,13 @@
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
       <c r="N118" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="O118" s="4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="P118" s="4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="Q118" s="4"/>
       <c r="R118" s="4"/>
@@ -8538,18 +8531,18 @@
         <v>393</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C119" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D119" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanDate")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/loanDate</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanForBotanist")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/loanForBotanist</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F119" s="4" t="s">
         <v>20</v>
@@ -8564,13 +8557,13 @@
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
       <c r="N119" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O119" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P119" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q119" s="4"/>
       <c r="R119" s="4"/>
@@ -8580,18 +8573,18 @@
         <v>393</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C120" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D120" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanReturnDate")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/loanReturnDate</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanDate")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/loanDate</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F120" s="4" t="s">
         <v>20</v>
@@ -8606,34 +8599,34 @@
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
       <c r="N120" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="O120" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="P120" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="Q120" s="4"/>
       <c r="R120" s="4"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>418</v>
+        <v>393</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C121" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D121" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitType")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitType</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/loanReturnDate")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/loanReturnDate</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F121" s="4" t="s">
         <v>20</v>
@@ -8641,17 +8634,21 @@
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
-      <c r="J121" s="4" t="s">
-        <v>421</v>
-      </c>
+      <c r="J121" s="4"/>
       <c r="K121" s="4" t="s">
-        <v>505</v>
+        <v>22</v>
       </c>
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
+      <c r="N121" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="O121" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="P121" s="4" t="s">
+        <v>417</v>
+      </c>
       <c r="Q121" s="4"/>
       <c r="R121" s="4"/>
     </row>
@@ -8660,18 +8657,18 @@
         <v>418</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C122" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D122" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitReferenceNumber")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitReferenceNumber</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitType")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitType</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F122" s="4" t="s">
         <v>20</v>
@@ -8679,7 +8676,9 @@
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
-      <c r="J122" s="4"/>
+      <c r="J122" s="4" t="s">
+        <v>421</v>
+      </c>
       <c r="K122" s="4" t="s">
         <v>505</v>
       </c>
@@ -8696,18 +8695,18 @@
         <v>418</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C123" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D123" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitIssuedBy")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitIssuedBy</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitReferenceNumber")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitReferenceNumber</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F123" s="4" t="s">
         <v>20</v>
@@ -8719,10 +8718,7 @@
       <c r="K123" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="L123" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
-        <v>https://github.com/hiscom/hispid/issues/10</v>
-      </c>
+      <c r="L123" s="4"/>
       <c r="M123" s="4"/>
       <c r="N123" s="4"/>
       <c r="O123" s="4"/>
@@ -8735,18 +8731,18 @@
         <v>418</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C124" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D124" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitIssuedTo")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitIssuedTo</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitIssuedBy")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitIssuedBy</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F124" s="4" t="s">
         <v>20</v>
@@ -8759,7 +8755,7 @@
         <v>505</v>
       </c>
       <c r="L124" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" ref="L124:L131" si="6">HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M124" s="4"/>
@@ -8774,21 +8770,21 @@
         <v>418</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C125" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D125" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitIssuedDate")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitIssuedDate</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitIssuedTo")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitIssuedTo</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
@@ -8798,7 +8794,7 @@
         <v>505</v>
       </c>
       <c r="L125" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M125" s="4"/>
@@ -8813,25 +8809,23 @@
         <v>418</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C126" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D126" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitValidDate")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitValidDate</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitIssuedDate")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitIssuedDate</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F126" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G126" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
@@ -8839,7 +8833,7 @@
         <v>505</v>
       </c>
       <c r="L126" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M126" s="4"/>
@@ -8849,39 +8843,38 @@
       <c r="Q126" s="4"/>
       <c r="R126" s="4"/>
     </row>
-    <row r="127" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>418</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C127" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D127" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitStatus")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitStatus</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitValidDate")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitValidDate</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G127" s="4"/>
-      <c r="H127" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/permit_status.xml")</f>
-        <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/permit_status.xml</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H127" s="4"/>
       <c r="I127" s="4"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4" t="s">
         <v>505</v>
       </c>
       <c r="L127" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M127" s="4"/>
@@ -8896,31 +8889,34 @@
         <v>418</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C128" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D128" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitConditions")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitConditions</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitStatus")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitStatus</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F128" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
+      <c r="H128" s="7" t="str">
+        <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/permit_status.xml")</f>
+        <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/permit_status.xml</v>
+      </c>
       <c r="I128" s="4"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4" t="s">
         <v>505</v>
       </c>
       <c r="L128" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M128" s="4"/>
@@ -8930,23 +8926,23 @@
       <c r="Q128" s="4"/>
       <c r="R128" s="4"/>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>418</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C129" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D129" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitRemarks")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitRemarks</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitConditions")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitConditions</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F129" s="4" t="s">
         <v>20</v>
@@ -8959,7 +8955,7 @@
         <v>505</v>
       </c>
       <c r="L129" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M129" s="4"/>
@@ -8974,18 +8970,18 @@
         <v>418</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C130" s="7" t="str">
         <f t="shared" si="5"/>
         <v>http://hiscom.chah.org.au/hispid/terms</v>
       </c>
       <c r="D130" s="7" t="str">
-        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitLink")</f>
-        <v>http://hiscom.chah.org.au/hispid/terms/permitLink</v>
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitRemarks")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitRemarks</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F130" s="4" t="s">
         <v>20</v>
@@ -8998,7 +8994,7 @@
         <v>505</v>
       </c>
       <c r="L130" s="7" t="str">
-        <f>HYPERLINK("https://github.com/hiscom/hispid/issues/10")</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/hiscom/hispid/issues/10</v>
       </c>
       <c r="M130" s="4"/>
@@ -9010,19 +9006,21 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>581</v>
+        <v>418</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>529</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>542</v>
+        <v>438</v>
+      </c>
+      <c r="C131" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hiscom.chah.org.au/hispid/terms</v>
+      </c>
+      <c r="D131" s="7" t="str">
+        <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/permitLink")</f>
+        <v>http://hiscom.chah.org.au/hispid/terms/permitLink</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>570</v>
+        <v>439</v>
       </c>
       <c r="F131" s="4" t="s">
         <v>20</v>
@@ -9032,40 +9030,39 @@
       <c r="I131" s="4"/>
       <c r="J131" s="4"/>
       <c r="K131" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="L131" s="4"/>
+        <v>505</v>
+      </c>
+      <c r="L131" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>https://github.com/hiscom/hispid/issues/10</v>
+      </c>
       <c r="M131" s="4"/>
       <c r="N131" s="4"/>
       <c r="O131" s="4"/>
       <c r="P131" s="4"/>
       <c r="Q131" s="4"/>
-      <c r="R131" s="4" t="s">
-        <v>663</v>
-      </c>
+      <c r="R131" s="4"/>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D132" s="7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G132" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
       <c r="J132" s="4"/>
@@ -9079,7 +9076,7 @@
       <c r="P132" s="4"/>
       <c r="Q132" s="4"/>
       <c r="R132" s="4" t="s">
-        <v>704</v>
+        <v>663</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
@@ -9087,16 +9084,16 @@
         <v>581</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>520</v>
+        <v>545</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F133" s="4" t="s">
         <v>28</v>
@@ -9117,31 +9114,31 @@
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
       <c r="R133" s="4" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>528</v>
-      </c>
-      <c r="C134" s="7" t="str">
-        <f>HYPERLINK("http://purl.org/dc/elements/1.1")</f>
-        <v>http://purl.org/dc/elements/1.1</v>
-      </c>
-      <c r="D134" s="7" t="str">
-        <f>HYPERLINK("http://purl.org/dc/elements/1.1/source")</f>
-        <v>http://purl.org/dc/elements/1.1/source</v>
+        <v>547</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>546</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G134" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="G134" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
       <c r="J134" s="4"/>
@@ -9155,24 +9152,26 @@
       <c r="P134" s="4"/>
       <c r="Q134" s="4"/>
       <c r="R134" s="4" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="D135" s="7" t="s">
-        <v>548</v>
+        <v>528</v>
+      </c>
+      <c r="C135" s="7" t="str">
+        <f>HYPERLINK("http://purl.org/dc/elements/1.1")</f>
+        <v>http://purl.org/dc/elements/1.1</v>
+      </c>
+      <c r="D135" s="7" t="str">
+        <f>HYPERLINK("http://purl.org/dc/elements/1.1/source")</f>
+        <v>http://purl.org/dc/elements/1.1/source</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="F135" s="4" t="s">
         <v>20</v>
@@ -9190,8 +9189,8 @@
       <c r="O135" s="4"/>
       <c r="P135" s="4"/>
       <c r="Q135" s="4"/>
-      <c r="R135" s="14" t="s">
-        <v>624</v>
+      <c r="R135" s="4" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
@@ -9199,16 +9198,16 @@
         <v>581</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>4</v>
+        <v>530</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>549</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>20</v>
@@ -9226,25 +9225,25 @@
       <c r="O136" s="4"/>
       <c r="P136" s="4"/>
       <c r="Q136" s="4"/>
-      <c r="R136" s="4" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="R136" s="14" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>531</v>
+        <v>4</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>520</v>
+        <v>549</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="F137" s="4" t="s">
         <v>20</v>
@@ -9263,32 +9262,30 @@
       <c r="P137" s="4"/>
       <c r="Q137" s="4"/>
       <c r="R137" s="4" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F138" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G138" s="4"/>
-      <c r="H138" s="4" t="s">
-        <v>563</v>
-      </c>
+      <c r="H138" s="4"/>
       <c r="I138" s="4"/>
       <c r="J138" s="4"/>
       <c r="K138" s="4" t="s">
@@ -9301,7 +9298,7 @@
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
       <c r="R138" s="4" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
@@ -9309,39 +9306,37 @@
         <v>581</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>553</v>
+        <v>520</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F139" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="L139" s="7" t="s">
-        <v>760</v>
-      </c>
+      <c r="L139" s="4"/>
       <c r="M139" s="4"/>
       <c r="N139" s="4"/>
       <c r="O139" s="4"/>
       <c r="P139" s="4"/>
       <c r="Q139" s="4"/>
       <c r="R139" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
@@ -9349,35 +9344,39 @@
         <v>581</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="F140" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
+      <c r="H140" s="4" t="s">
+        <v>564</v>
+      </c>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="L140" s="4"/>
+      <c r="L140" s="7" t="s">
+        <v>758</v>
+      </c>
       <c r="M140" s="4"/>
       <c r="N140" s="4"/>
       <c r="O140" s="4"/>
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
       <c r="R140" s="4" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
@@ -9385,16 +9384,16 @@
         <v>581</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F141" s="4" t="s">
         <v>20</v>
@@ -9413,24 +9412,24 @@
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>
       <c r="R141" s="4" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="F142" s="4" t="s">
         <v>20</v>
@@ -9449,24 +9448,24 @@
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
       <c r="R142" s="4" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F143" s="4" t="s">
         <v>20</v>
@@ -9485,7 +9484,7 @@
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
       <c r="R143" s="4" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
@@ -9493,16 +9492,16 @@
         <v>581</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F144" s="4" t="s">
         <v>20</v>
@@ -9521,7 +9520,7 @@
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
       <c r="R144" s="4" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
@@ -9529,16 +9528,16 @@
         <v>581</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F145" s="4" t="s">
         <v>20</v>
@@ -9557,24 +9556,24 @@
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
       <c r="R145" s="4" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>618</v>
+        <v>539</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>549</v>
+        <v>520</v>
       </c>
       <c r="D146" s="7" t="s">
-        <v>619</v>
+        <v>560</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>620</v>
+        <v>580</v>
       </c>
       <c r="F146" s="4" t="s">
         <v>20</v>
@@ -9593,34 +9592,30 @@
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
       <c r="R146" s="4" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>520</v>
+        <v>549</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="F147" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G147" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="H147" s="4" t="s">
-        <v>628</v>
-      </c>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4" t="s">
@@ -9633,32 +9628,34 @@
       <c r="P147" s="4"/>
       <c r="Q147" s="4"/>
       <c r="R147" s="4" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
       <c r="D148" s="7" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G148" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="H148" s="4"/>
+        <v>627</v>
+      </c>
+      <c r="H148" s="4" t="s">
+        <v>628</v>
+      </c>
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
       <c r="K148" s="4" t="s">
@@ -9671,29 +9668,31 @@
       <c r="P148" s="4"/>
       <c r="Q148" s="4"/>
       <c r="R148" s="4" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>520</v>
+        <v>545</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="E149" s="14" t="s">
-        <v>636</v>
+        <v>630</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>631</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G149" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="G149" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
@@ -9707,31 +9706,29 @@
       <c r="P149" s="4"/>
       <c r="Q149" s="4"/>
       <c r="R149" s="4" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>17</v>
+        <v>581</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>549</v>
+        <v>520</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>639</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>640</v>
+        <v>635</v>
+      </c>
+      <c r="E150" s="14" t="s">
+        <v>636</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G150" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
       <c r="J150" s="4"/>
@@ -9745,7 +9742,7 @@
       <c r="P150" s="4"/>
       <c r="Q150" s="4"/>
       <c r="R150" s="4" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
@@ -9753,21 +9750,23 @@
         <v>581</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>520</v>
+        <v>549</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G151" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="G151" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
@@ -9781,24 +9780,24 @@
       <c r="P151" s="4"/>
       <c r="Q151" s="4"/>
       <c r="R151" s="4" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="152" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>17</v>
+        <v>581</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>549</v>
+        <v>520</v>
       </c>
       <c r="D152" s="7" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>20</v>
@@ -9817,24 +9816,24 @@
       <c r="P152" s="4"/>
       <c r="Q152" s="4"/>
       <c r="R152" s="4" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="D153" s="7" t="s">
-        <v>676</v>
+        <v>647</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>677</v>
+        <v>648</v>
       </c>
       <c r="F153" s="4" t="s">
         <v>20</v>
@@ -9853,24 +9852,24 @@
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
       <c r="R153" s="4" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="154" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C154" s="7" t="s">
         <v>545</v>
       </c>
       <c r="D154" s="7" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F154" s="4" t="s">
         <v>20</v>
@@ -9889,24 +9888,24 @@
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
       <c r="R154" s="4" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>520</v>
+        <v>545</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F155" s="4" t="s">
         <v>20</v>
@@ -9925,7 +9924,7 @@
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
       <c r="R155" s="4" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
@@ -9933,16 +9932,16 @@
         <v>581</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>674</v>
+        <v>520</v>
       </c>
       <c r="D156" s="7" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F156" s="4" t="s">
         <v>20</v>
@@ -9961,7 +9960,7 @@
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
       <c r="R156" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
@@ -9969,16 +9968,16 @@
         <v>581</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>520</v>
+        <v>674</v>
       </c>
       <c r="D157" s="7" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F157" s="4" t="s">
         <v>20</v>
@@ -9997,24 +9996,24 @@
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
       <c r="R157" s="4" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="158" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D158" s="7" t="s">
-        <v>683</v>
+        <v>672</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F158" s="4" t="s">
         <v>20</v>
@@ -10033,24 +10032,24 @@
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
       <c r="R158" s="4" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="F159" s="4" t="s">
         <v>20</v>
@@ -10069,7 +10068,7 @@
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
       <c r="R159" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
@@ -10077,16 +10076,16 @@
         <v>581</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="F160" s="4" t="s">
         <v>20</v>
@@ -10105,24 +10104,24 @@
       <c r="P160" s="4"/>
       <c r="Q160" s="4"/>
       <c r="R160" s="4" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>581</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>694</v>
+        <v>664</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D161" s="7" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="F161" s="4" t="s">
         <v>20</v>
@@ -10140,8 +10139,8 @@
       <c r="O161" s="4"/>
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
-      <c r="R161" s="15" t="s">
-        <v>697</v>
+      <c r="R161" s="4" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="162" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -10149,16 +10148,16 @@
         <v>581</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D162" s="7" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
       <c r="F162" s="4" t="s">
         <v>20</v>
@@ -10176,25 +10175,25 @@
       <c r="O162" s="4"/>
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
-      <c r="R162" s="4" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R162" s="15" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>268</v>
+        <v>581</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="D163" s="7" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="F163" s="4" t="s">
         <v>20</v>
@@ -10213,22 +10212,24 @@
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
       <c r="R163" s="4" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A164" s="4"/>
+      <c r="A164" s="4" t="s">
+        <v>581</v>
+      </c>
       <c r="B164" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D164" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="E164" s="4" t="s">
         <v>728</v>
-      </c>
-      <c r="E164" s="4" t="s">
-        <v>729</v>
       </c>
       <c r="F164" s="4" t="s">
         <v>20</v>
@@ -10247,7 +10248,7 @@
       <c r="P164" s="4"/>
       <c r="Q164" s="4"/>
       <c r="R164" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="165" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -10255,22 +10256,22 @@
         <v>581</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D165" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="E165" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="E165" s="4" t="s">
+      <c r="F165" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G165" s="4" t="s">
         <v>733</v>
-      </c>
-      <c r="F165" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G165" s="4" t="s">
-        <v>734</v>
       </c>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
@@ -10285,7 +10286,7 @@
       <c r="P165" s="4"/>
       <c r="Q165" s="4"/>
       <c r="R165" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
@@ -10293,16 +10294,16 @@
         <v>581</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C166" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D166" s="7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F166" s="4" t="s">
         <v>20</v>
@@ -10321,24 +10322,24 @@
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
       <c r="R166" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="167" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>750</v>
+        <v>581</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D167" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>741</v>
-      </c>
-      <c r="E167" s="4" t="s">
-        <v>742</v>
       </c>
       <c r="F167" s="4" t="s">
         <v>20</v>
@@ -10357,34 +10358,34 @@
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
       <c r="R167" s="4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="168" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>750</v>
+        <v>581</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>543</v>
       </c>
       <c r="D168" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F168" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G168" s="4"/>
       <c r="H168" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="I168" s="4" t="s">
         <v>747</v>
-      </c>
-      <c r="I168" s="4" t="s">
-        <v>748</v>
       </c>
       <c r="J168" s="4"/>
       <c r="K168" s="4" t="s">
@@ -10397,24 +10398,24 @@
       <c r="P168" s="4"/>
       <c r="Q168" s="4"/>
       <c r="R168" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="169" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>750</v>
+        <v>581</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D169" s="7" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F169" s="4" t="s">
         <v>20</v>
@@ -10433,24 +10434,24 @@
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
       <c r="R169" s="4" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="170" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>750</v>
+        <v>581</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>520</v>
       </c>
       <c r="D170" s="7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F170" s="4" t="s">
         <v>20</v>
@@ -10469,7 +10470,7 @@
       <c r="P170" s="4"/>
       <c r="Q170" s="4"/>
       <c r="R170" s="4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
@@ -10839,7 +10840,7 @@
     <hyperlink ref="H17" r:id="rId3" display="https://github.com/hiscom/hispid-review-2014-15/issues/22"/>
     <hyperlink ref="H19" r:id="rId4"/>
     <hyperlink ref="H87" r:id="rId5"/>
-    <hyperlink ref="H98" r:id="rId6"/>
+    <hyperlink ref="H99" r:id="rId6"/>
     <hyperlink ref="N58" r:id="rId7" display="http://wiki.tdwg.org/twiki/bin/view/ABCD/AbcdConcept1121"/>
     <hyperlink ref="C21" r:id="rId8"/>
     <hyperlink ref="D21" r:id="rId9"/>
@@ -10852,73 +10853,73 @@
     <hyperlink ref="D8" r:id="rId16" display="http://ns.adobe.com/xap/1.0/rights/Owner"/>
     <hyperlink ref="C9" r:id="rId17" display="http://ns.adobe.com/xap/1.0/rights"/>
     <hyperlink ref="D9" r:id="rId18" display="http://ns.adobe.com/xap/1.0/rights/WebStatement"/>
-    <hyperlink ref="C131" r:id="rId19"/>
-    <hyperlink ref="D131" r:id="rId20"/>
-    <hyperlink ref="C132" r:id="rId21"/>
-    <hyperlink ref="D132" r:id="rId22"/>
-    <hyperlink ref="C133" r:id="rId23"/>
-    <hyperlink ref="D133" r:id="rId24"/>
-    <hyperlink ref="C135" r:id="rId25"/>
-    <hyperlink ref="D135" r:id="rId26"/>
-    <hyperlink ref="C136" r:id="rId27"/>
-    <hyperlink ref="D136" r:id="rId28"/>
-    <hyperlink ref="C137" r:id="rId29"/>
-    <hyperlink ref="D137" r:id="rId30"/>
-    <hyperlink ref="C138" r:id="rId31"/>
-    <hyperlink ref="D138" r:id="rId32"/>
-    <hyperlink ref="C141" r:id="rId33"/>
-    <hyperlink ref="C139" r:id="rId34"/>
-    <hyperlink ref="D139" r:id="rId35"/>
-    <hyperlink ref="C140" r:id="rId36"/>
-    <hyperlink ref="D140" r:id="rId37"/>
-    <hyperlink ref="D141" r:id="rId38"/>
-    <hyperlink ref="C142" r:id="rId39"/>
-    <hyperlink ref="D142" r:id="rId40"/>
-    <hyperlink ref="C143" r:id="rId41"/>
-    <hyperlink ref="D143" r:id="rId42"/>
-    <hyperlink ref="C144" r:id="rId43"/>
-    <hyperlink ref="D144" r:id="rId44"/>
-    <hyperlink ref="C145" r:id="rId45"/>
-    <hyperlink ref="D145" r:id="rId46"/>
+    <hyperlink ref="C132" r:id="rId19"/>
+    <hyperlink ref="D132" r:id="rId20"/>
+    <hyperlink ref="C133" r:id="rId21"/>
+    <hyperlink ref="D133" r:id="rId22"/>
+    <hyperlink ref="C134" r:id="rId23"/>
+    <hyperlink ref="D134" r:id="rId24"/>
+    <hyperlink ref="C136" r:id="rId25"/>
+    <hyperlink ref="D136" r:id="rId26"/>
+    <hyperlink ref="C137" r:id="rId27"/>
+    <hyperlink ref="D137" r:id="rId28"/>
+    <hyperlink ref="C138" r:id="rId29"/>
+    <hyperlink ref="D138" r:id="rId30"/>
+    <hyperlink ref="C139" r:id="rId31"/>
+    <hyperlink ref="D139" r:id="rId32"/>
+    <hyperlink ref="C142" r:id="rId33"/>
+    <hyperlink ref="C140" r:id="rId34"/>
+    <hyperlink ref="D140" r:id="rId35"/>
+    <hyperlink ref="C141" r:id="rId36"/>
+    <hyperlink ref="D141" r:id="rId37"/>
+    <hyperlink ref="D142" r:id="rId38"/>
+    <hyperlink ref="C143" r:id="rId39"/>
+    <hyperlink ref="D143" r:id="rId40"/>
+    <hyperlink ref="C144" r:id="rId41"/>
+    <hyperlink ref="D144" r:id="rId42"/>
+    <hyperlink ref="C145" r:id="rId43"/>
+    <hyperlink ref="D145" r:id="rId44"/>
+    <hyperlink ref="C146" r:id="rId45"/>
+    <hyperlink ref="D146" r:id="rId46"/>
     <hyperlink ref="H14" r:id="rId47" display="https://github.com/hiscom/hispid-review-2014-15/issues/22"/>
-    <hyperlink ref="L139" r:id="rId48" display="https://www.google.com/url?q=https%3A%2F%2Fgithub.com%2Fhiscom%2Fhispid-review-2014-15%2Fissues%2F5&amp;sa=D&amp;sntz=1&amp;usg=AFQjCNHeqJd4V7be2Ny-Dge3p9KxCsLqgg"/>
+    <hyperlink ref="L140" r:id="rId48" display="https://www.google.com/url?q=https%3A%2F%2Fgithub.com%2Fhiscom%2Fhispid-review-2014-15%2Fissues%2F5&amp;sa=D&amp;sntz=1&amp;usg=AFQjCNHeqJd4V7be2Ny-Dge3p9KxCsLqgg"/>
     <hyperlink ref="D18" r:id="rId49"/>
-    <hyperlink ref="C146" r:id="rId50"/>
-    <hyperlink ref="D146" r:id="rId51"/>
-    <hyperlink ref="C147" r:id="rId52"/>
-    <hyperlink ref="D147" r:id="rId53"/>
-    <hyperlink ref="D148" r:id="rId54"/>
-    <hyperlink ref="C148" r:id="rId55"/>
-    <hyperlink ref="C149" r:id="rId56"/>
-    <hyperlink ref="D149" r:id="rId57"/>
-    <hyperlink ref="D150" r:id="rId58"/>
-    <hyperlink ref="C150" r:id="rId59"/>
-    <hyperlink ref="C151" r:id="rId60"/>
-    <hyperlink ref="D151" r:id="rId61"/>
-    <hyperlink ref="D152" r:id="rId62"/>
-    <hyperlink ref="C152" r:id="rId63"/>
-    <hyperlink ref="C157" r:id="rId64"/>
-    <hyperlink ref="D155" r:id="rId65"/>
-    <hyperlink ref="C155" r:id="rId66"/>
-    <hyperlink ref="D157" r:id="rId67"/>
-    <hyperlink ref="D156" r:id="rId68"/>
-    <hyperlink ref="C156" r:id="rId69"/>
-    <hyperlink ref="D154" r:id="rId70"/>
-    <hyperlink ref="C154" r:id="rId71"/>
-    <hyperlink ref="D153" r:id="rId72"/>
-    <hyperlink ref="C153" r:id="rId73"/>
-    <hyperlink ref="D158" r:id="rId74"/>
-    <hyperlink ref="C158" r:id="rId75"/>
-    <hyperlink ref="D159" r:id="rId76"/>
-    <hyperlink ref="C159" r:id="rId77"/>
-    <hyperlink ref="D160" r:id="rId78"/>
-    <hyperlink ref="C160" r:id="rId79"/>
-    <hyperlink ref="C161" r:id="rId80"/>
-    <hyperlink ref="D161" r:id="rId81"/>
-    <hyperlink ref="C162" r:id="rId82"/>
-    <hyperlink ref="D162" r:id="rId83"/>
-    <hyperlink ref="D163" r:id="rId84"/>
-    <hyperlink ref="C163" r:id="rId85"/>
+    <hyperlink ref="C147" r:id="rId50"/>
+    <hyperlink ref="D147" r:id="rId51"/>
+    <hyperlink ref="C148" r:id="rId52"/>
+    <hyperlink ref="D148" r:id="rId53"/>
+    <hyperlink ref="D149" r:id="rId54"/>
+    <hyperlink ref="C149" r:id="rId55"/>
+    <hyperlink ref="C150" r:id="rId56"/>
+    <hyperlink ref="D150" r:id="rId57"/>
+    <hyperlink ref="D151" r:id="rId58"/>
+    <hyperlink ref="C151" r:id="rId59"/>
+    <hyperlink ref="C152" r:id="rId60"/>
+    <hyperlink ref="D152" r:id="rId61"/>
+    <hyperlink ref="D153" r:id="rId62"/>
+    <hyperlink ref="C153" r:id="rId63"/>
+    <hyperlink ref="C158" r:id="rId64"/>
+    <hyperlink ref="D156" r:id="rId65"/>
+    <hyperlink ref="C156" r:id="rId66"/>
+    <hyperlink ref="D158" r:id="rId67"/>
+    <hyperlink ref="D157" r:id="rId68"/>
+    <hyperlink ref="C157" r:id="rId69"/>
+    <hyperlink ref="D155" r:id="rId70"/>
+    <hyperlink ref="C155" r:id="rId71"/>
+    <hyperlink ref="D154" r:id="rId72"/>
+    <hyperlink ref="C154" r:id="rId73"/>
+    <hyperlink ref="D159" r:id="rId74"/>
+    <hyperlink ref="C159" r:id="rId75"/>
+    <hyperlink ref="D160" r:id="rId76"/>
+    <hyperlink ref="C160" r:id="rId77"/>
+    <hyperlink ref="D161" r:id="rId78"/>
+    <hyperlink ref="C161" r:id="rId79"/>
+    <hyperlink ref="C162" r:id="rId80"/>
+    <hyperlink ref="D162" r:id="rId81"/>
+    <hyperlink ref="C163" r:id="rId82"/>
+    <hyperlink ref="D163" r:id="rId83"/>
+    <hyperlink ref="D96" r:id="rId84"/>
+    <hyperlink ref="C96" r:id="rId85"/>
     <hyperlink ref="C164" r:id="rId86"/>
     <hyperlink ref="D164" r:id="rId87"/>
     <hyperlink ref="C165" r:id="rId88"/>

</xml_diff>

<commit_message>
Added dwc:parentEventID and dwc:eventID
</commit_message>
<xml_diff>
--- a/HISPID2015.xlsx
+++ b/HISPID2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HISPID2015" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="802">
   <si>
     <t>group</t>
   </si>
@@ -1538,9 +1538,6 @@
     <t>lifeStage</t>
   </si>
   <si>
-    <t>http://rs.tdwg.org/dwc/terms</t>
-  </si>
-  <si>
     <t>http://rs.tdwg.org/dwc/terms/lifeStage</t>
   </si>
   <si>
@@ -1646,9 +1643,6 @@
     <t>http://purl.org/dc/terms/title</t>
   </si>
   <si>
-    <t>http://purl.org/dc/terms</t>
-  </si>
-  <si>
     <t>http://purl.org/dc/terms/description</t>
   </si>
   <si>
@@ -2300,9 +2294,6 @@
     <t>http://hiscom.chah.org.au/hispid/terms/MediaItem</t>
   </si>
   <si>
-    <t>http://hiscom.chah.org.au/hispid/terms</t>
-  </si>
-  <si>
     <t>PreservedSpecimen</t>
   </si>
   <si>
@@ -2436,6 +2427,9 @@
   </si>
   <si>
     <t>organismQuantityType  must be delivered alongside this term. Note that this is a considerable deviation from earlier versions of HISPID, where Frequency was a free text field.</t>
+  </si>
+  <si>
+    <t>http://hiscom.chah.org.au/hispid/terms/</t>
   </si>
 </sst>
 </file>
@@ -3366,8 +3360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C153" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
@@ -3449,10 +3443,10 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -3534,10 +3528,10 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>22</v>
@@ -3607,7 +3601,7 @@
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="S4" s="17">
         <v>42196</v>
@@ -3678,7 +3672,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C6" s="6" t="str">
         <f>HYPERLINK("http://purl.org/dc/terms/")</f>
@@ -3714,7 +3708,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="S6" s="17">
         <v>42196</v>
@@ -3728,7 +3722,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C7" s="6" t="str">
         <f>HYPERLINK("http://purl.org/dc/terms/")</f>
@@ -3739,34 +3733,34 @@
         <v>http://purl.org/dc/terms/language</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>263</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="S7" s="17">
         <v>42196</v>
@@ -3780,7 +3774,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C8" s="6" t="str">
         <f>HYPERLINK("http://purl.org/dc/terms/")</f>
@@ -3791,7 +3785,7 @@
         <v>http://purl.org/dc/terms/rightsHolder</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>20</v>
@@ -3810,7 +3804,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="S8" s="17">
         <v>42196</v>
@@ -3824,7 +3818,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C9" s="6" t="str">
         <f>HYPERLINK("http://purl.org/dc/terms/")</f>
@@ -3835,7 +3829,7 @@
         <v>http://purl.org/dc/terms/license</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>20</v>
@@ -3844,7 +3838,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="8" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>263</v>
@@ -3856,7 +3850,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="S9" s="17">
         <v>42196</v>
@@ -3870,17 +3864,17 @@
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C10" s="6" t="str">
         <f t="shared" ref="C10:C11" si="0">HYPERLINK("http://rs.tdwg.org/dwc/terms/")</f>
         <v>http://rs.tdwg.org/dwc/terms/</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>20</v>
@@ -3889,19 +3883,19 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="8" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>263</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -3919,17 +3913,17 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>http://rs.tdwg.org/dwc/terms/</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>20</v>
@@ -3938,16 +3932,16 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="8" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>263</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -3983,7 +3977,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -4001,7 +3995,7 @@
         <v>41</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -4092,7 +4086,7 @@
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="9" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>51</v>
@@ -4191,7 +4185,7 @@
         <v>http://rs.tdwg.org/dwc/terms/preparations</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>20</v>
@@ -4203,7 +4197,7 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>22</v>
@@ -4226,7 +4220,7 @@
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="S16" s="17">
         <v>42196</v>
@@ -4261,7 +4255,7 @@
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="9" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
@@ -4315,7 +4309,7 @@
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
@@ -4368,20 +4362,20 @@
         <v>20</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H19" s="6" t="str">
         <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/organism_quantity.xml")</f>
         <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/organism_quantity.xml</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>68</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L19" s="6" t="str">
         <f>HYPERLINK("https://github.com/hiscom/hispid/issues/22")</f>
@@ -4415,17 +4409,17 @@
         <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C20" s="6" t="str">
         <f t="shared" si="1"/>
         <v>http://rs.tdwg.org/dwc/terms/</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>20</v>
@@ -4434,17 +4428,17 @@
       <c r="H20" s="6"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L20" s="6" t="str">
         <f>HYPERLINK("https://github.com/hiscom/hispid/issues/22")</f>
         <v>https://github.com/hiscom/hispid/issues/22</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -4574,13 +4568,13 @@
         <v>503</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>505</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>506</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>20</v>
@@ -4607,7 +4601,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="S23" s="17">
         <v>42196</v>
@@ -4621,16 +4615,16 @@
         <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>770</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>773</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>512</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>513</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>20</v>
@@ -4647,16 +4641,16 @@
         <v>https://github.com/hiscom/hispid/issues/34</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="S24" s="17">
         <v>42196</v>
@@ -4804,14 +4798,14 @@
         <v>20</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="H27" s="6" t="str">
         <f>HYPERLINK("http://hiscom.rbg.vic.gov.au/hispid/vocabulary/association_type.xml")</f>
         <v>http://hiscom.rbg.vic.gov.au/hispid/vocabulary/association_type.xml</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
@@ -4888,7 +4882,7 @@
         <v>40</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C29" s="6" t="str">
         <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/")</f>
@@ -4899,7 +4893,7 @@
         <v>http://rs.tdwg.org/dwc/terms/disposition</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>20</v>
@@ -4908,7 +4902,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>263</v>
@@ -4935,7 +4929,7 @@
         <v>90</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/")</f>
@@ -4946,13 +4940,13 @@
         <v>http://rs.tdwg.org/dwc/terms/eventID</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -4965,10 +4959,10 @@
         <v>https://github.com/hiscom/hispid/issues/2</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
@@ -4982,7 +4976,7 @@
         <v>90</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C31" s="6" t="str">
         <f>HYPERLINK("http://rs.tdwg.org/dwc/terms/")</f>
@@ -4993,13 +4987,13 @@
         <v>http://rs.tdwg.org/dwc/terms/parentEventID</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -5012,7 +5006,7 @@
         <v>https://github.com/hiscom/hispid/issues/75</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -5403,7 +5397,7 @@
         <v>http://rs.tdwg.org/dwc/terms/eventDate</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>118</v>
@@ -5434,7 +5428,7 @@
       </c>
       <c r="Q39" s="4"/>
       <c r="R39" s="4" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="S39" s="17">
         <v>42196</v>
@@ -5498,7 +5492,7 @@
         <v>90</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C41" s="6" t="str">
         <f>HYPERLINK("http://hiscom.chah.org.au/hispid/terms/")</f>
@@ -5509,7 +5503,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/collectingTrip</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>20</v>
@@ -5631,7 +5625,7 @@
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="4" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="S43" s="17">
         <v>42196</v>
@@ -5712,7 +5706,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="13" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>139</v>
@@ -5735,7 +5729,7 @@
       </c>
       <c r="Q45" s="4"/>
       <c r="R45" s="4" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="S45" s="17">
         <v>42196</v>
@@ -5791,7 +5785,7 @@
       </c>
       <c r="Q46" s="4"/>
       <c r="R46" s="4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="S46" s="17">
         <v>42196</v>
@@ -5847,7 +5841,7 @@
         <v>461</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="S47" s="17">
         <v>42196</v>
@@ -6198,7 +6192,7 @@
       </c>
       <c r="O54" s="4"/>
       <c r="P54" s="4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
@@ -6399,7 +6393,7 @@
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>500</v>
@@ -6696,7 +6690,7 @@
         <v>http://rs.tdwg.org/dwc/terms/georeferencedDate</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>20</v>
@@ -6744,7 +6738,7 @@
         <v>http://rs.tdwg.org/dwc/terms/georeferenceSources</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>20</v>
@@ -7357,7 +7351,7 @@
       </c>
       <c r="Q77" s="4"/>
       <c r="R77" s="4" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="S77" s="17">
         <v>42196</v>
@@ -7481,7 +7475,7 @@
         <v>http://rs.tdwg.org/dwc/terms/identificationVerificationStatus</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>20</v>
@@ -7615,7 +7609,7 @@
       </c>
       <c r="Q82" s="4"/>
       <c r="R82" s="4" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="S82" s="17">
         <v>42196</v>
@@ -7667,7 +7661,7 @@
       </c>
       <c r="Q83" s="4"/>
       <c r="R83" s="4" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="S83" s="17">
         <v>42196</v>
@@ -8483,16 +8477,16 @@
         <v>315</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="F100" s="4" t="s">
         <v>20</v>
@@ -8506,14 +8500,14 @@
       </c>
       <c r="L100" s="4"/>
       <c r="M100" s="4" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="N100" s="4"/>
       <c r="O100" s="4"/>
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
       <c r="R100" s="4" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="S100" s="17">
         <v>42196</v>
@@ -8567,7 +8561,7 @@
       </c>
       <c r="Q101" s="4"/>
       <c r="R101" s="4" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="S101" s="17">
         <v>42196</v>
@@ -8703,7 +8697,7 @@
         <v>263</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="M104" s="4" t="s">
         <v>359</v>
@@ -8769,7 +8763,7 @@
       </c>
       <c r="Q105" s="4"/>
       <c r="R105" s="4" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="S105" s="17">
         <v>42196</v>
@@ -8933,7 +8927,7 @@
         <v>315</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C109" s="6" t="str">
         <f t="shared" si="5"/>
@@ -8944,7 +8938,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/hybridFlag</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F109" s="4" t="s">
         <v>20</v>
@@ -8952,7 +8946,7 @@
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="J109" s="4"/>
       <c r="K109" s="4" t="s">
@@ -8984,7 +8978,7 @@
         <v>315</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C110" s="6" t="str">
         <f t="shared" si="5"/>
@@ -8995,7 +8989,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/hybridParent1</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F110" s="4" t="s">
         <v>20</v>
@@ -9029,7 +9023,7 @@
         <v>315</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C111" s="6" t="str">
         <f t="shared" si="5"/>
@@ -9040,7 +9034,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/hybridParent2</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F111" s="4" t="s">
         <v>20</v>
@@ -9075,7 +9069,7 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>376</v>
@@ -9126,10 +9120,10 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C113" s="6" t="str">
         <f t="shared" si="5"/>
@@ -9140,7 +9134,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/exsiccataSeries</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
@@ -9151,7 +9145,7 @@
         <v>500</v>
       </c>
       <c r="L113" s="6" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M113" s="4"/>
       <c r="N113" s="4"/>
@@ -9168,10 +9162,10 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C114" s="6" t="str">
         <f t="shared" si="5"/>
@@ -9182,7 +9176,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/exsiccataFascicle</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
@@ -9193,7 +9187,7 @@
         <v>500</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M114" s="4"/>
       <c r="N114" s="4"/>
@@ -9210,10 +9204,10 @@
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C115" s="6" t="str">
         <f t="shared" si="5"/>
@@ -9224,7 +9218,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/exsiccataNumber</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
@@ -9235,7 +9229,7 @@
         <v>500</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M115" s="4"/>
       <c r="N115" s="4"/>
@@ -9252,10 +9246,10 @@
     </row>
     <row r="116" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C116" s="6" t="str">
         <f t="shared" si="5"/>
@@ -9266,7 +9260,7 @@
         <v>http://hiscom.chah.org.au/hispid/terms/voucherFor</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F116" s="4" t="s">
         <v>20</v>
@@ -9303,7 +9297,7 @@
     </row>
     <row r="117" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>381</v>
@@ -9335,7 +9329,7 @@
         <v>22</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="M117" s="4"/>
       <c r="N117" s="4" t="s">
@@ -9360,7 +9354,7 @@
     </row>
     <row r="118" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>385</v>
@@ -10202,19 +10196,19 @@
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>20</v>
@@ -10236,7 +10230,7 @@
       <c r="P136" s="4"/>
       <c r="Q136" s="4"/>
       <c r="R136" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="S136" s="17">
         <v>42196</v>
@@ -10247,19 +10241,19 @@
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F137" s="4" t="s">
         <v>28</v>
@@ -10280,7 +10274,7 @@
       <c r="P137" s="4"/>
       <c r="Q137" s="4"/>
       <c r="R137" s="4" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="S137" s="17">
         <v>42196</v>
@@ -10291,19 +10285,19 @@
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F138" s="4" t="s">
         <v>28</v>
@@ -10324,7 +10318,7 @@
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
       <c r="R138" s="4" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="S138" s="17">
         <v>42196</v>
@@ -10335,10 +10329,10 @@
     </row>
     <row r="139" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C139" s="6" t="str">
         <f>HYPERLINK("http://purl.org/dc/elements/1.1/")</f>
@@ -10349,7 +10343,7 @@
         <v>http://purl.org/dc/elements/1.1/source</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F139" s="4" t="s">
         <v>20</v>
@@ -10368,7 +10362,7 @@
       <c r="P139" s="4"/>
       <c r="Q139" s="4"/>
       <c r="R139" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="S139" s="17">
         <v>42196</v>
@@ -10379,19 +10373,19 @@
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F140" s="4" t="s">
         <v>20</v>
@@ -10410,7 +10404,7 @@
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
       <c r="R140" s="13" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="S140" s="17">
         <v>42196</v>
@@ -10421,19 +10415,19 @@
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F141" s="4" t="s">
         <v>20</v>
@@ -10452,7 +10446,7 @@
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>
       <c r="R141" s="4" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="S141" s="17">
         <v>42196</v>
@@ -10463,19 +10457,19 @@
     </row>
     <row r="142" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F142" s="4" t="s">
         <v>20</v>
@@ -10494,7 +10488,7 @@
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
       <c r="R142" s="4" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="S142" s="17">
         <v>42196</v>
@@ -10505,26 +10499,26 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F143" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G143" s="4"/>
       <c r="H143" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
@@ -10538,7 +10532,7 @@
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
       <c r="R143" s="4" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="S143" s="17">
         <v>42196</v>
@@ -10549,26 +10543,26 @@
     </row>
     <row r="144" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F144" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="I144" s="4"/>
       <c r="J144" s="4"/>
@@ -10576,7 +10570,7 @@
         <v>263</v>
       </c>
       <c r="L144" s="6" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="M144" s="4"/>
       <c r="N144" s="4"/>
@@ -10584,7 +10578,7 @@
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
       <c r="R144" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="S144" s="17">
         <v>42196</v>
@@ -10595,19 +10589,19 @@
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F145" s="4" t="s">
         <v>20</v>
@@ -10626,7 +10620,7 @@
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
       <c r="R145" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="S145" s="17">
         <v>42196</v>
@@ -10637,19 +10631,19 @@
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F146" s="4" t="s">
         <v>20</v>
@@ -10668,7 +10662,7 @@
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
       <c r="R146" s="4" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="S146" s="17">
         <v>42196</v>
@@ -10679,19 +10673,19 @@
     </row>
     <row r="147" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F147" s="4" t="s">
         <v>20</v>
@@ -10710,7 +10704,7 @@
       <c r="P147" s="4"/>
       <c r="Q147" s="4"/>
       <c r="R147" s="4" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="S147" s="17">
         <v>42196</v>
@@ -10721,19 +10715,19 @@
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F148" s="4" t="s">
         <v>20</v>
@@ -10752,7 +10746,7 @@
       <c r="P148" s="4"/>
       <c r="Q148" s="4"/>
       <c r="R148" s="4" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="S148" s="17">
         <v>42196</v>
@@ -10763,19 +10757,19 @@
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F149" s="4" t="s">
         <v>20</v>
@@ -10794,7 +10788,7 @@
       <c r="P149" s="4"/>
       <c r="Q149" s="4"/>
       <c r="R149" s="4" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="S149" s="17">
         <v>42196</v>
@@ -10805,19 +10799,19 @@
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F150" s="4" t="s">
         <v>20</v>
@@ -10836,7 +10830,7 @@
       <c r="P150" s="4"/>
       <c r="Q150" s="4"/>
       <c r="R150" s="4" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="S150" s="17">
         <v>42196</v>
@@ -10847,19 +10841,19 @@
     </row>
     <row r="151" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B151" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="E151" s="4" t="s">
         <v>607</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>774</v>
-      </c>
-      <c r="D151" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="E151" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="F151" s="4" t="s">
         <v>20</v>
@@ -10878,7 +10872,7 @@
       <c r="P151" s="4"/>
       <c r="Q151" s="4"/>
       <c r="R151" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="S151" s="17">
         <v>42196</v>
@@ -10889,28 +10883,28 @@
     </row>
     <row r="152" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D152" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="F152" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G152" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="E152" s="4" t="s">
+      <c r="H152" s="4" t="s">
         <v>615</v>
-      </c>
-      <c r="F152" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G152" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="H152" s="4" t="s">
-        <v>617</v>
       </c>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
@@ -10927,7 +10921,7 @@
       <c r="P152" s="4"/>
       <c r="Q152" s="4"/>
       <c r="R152" s="4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="S152" s="17">
         <v>42196</v>
@@ -10938,19 +10932,19 @@
     </row>
     <row r="153" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B153" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="E153" s="4" t="s">
         <v>618</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>776</v>
-      </c>
-      <c r="D153" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E153" s="4" t="s">
-        <v>620</v>
       </c>
       <c r="F153" s="4" t="s">
         <v>28</v>
@@ -10971,7 +10965,7 @@
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
       <c r="R153" s="4" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="S153" s="17">
         <v>42196</v>
@@ -10982,19 +10976,19 @@
     </row>
     <row r="154" spans="1:20" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B154" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D154" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="E154" s="13" t="s">
         <v>623</v>
-      </c>
-      <c r="C154" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>624</v>
-      </c>
-      <c r="E154" s="13" t="s">
-        <v>625</v>
       </c>
       <c r="F154" s="4" t="s">
         <v>20</v>
@@ -11013,7 +11007,7 @@
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
       <c r="R154" s="4" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="S154" s="17">
         <v>42196</v>
@@ -11024,19 +11018,19 @@
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B155" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="D155" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="E155" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="C155" s="6" t="s">
-        <v>774</v>
-      </c>
-      <c r="D155" s="6" t="s">
-        <v>628</v>
-      </c>
-      <c r="E155" s="4" t="s">
-        <v>629</v>
       </c>
       <c r="F155" s="4" t="s">
         <v>28</v>
@@ -11057,7 +11051,7 @@
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
       <c r="R155" s="4" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="S155" s="17">
         <v>42196</v>
@@ -11068,19 +11062,19 @@
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B156" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>630</v>
+      </c>
+      <c r="E156" s="4" t="s">
         <v>631</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>632</v>
-      </c>
-      <c r="E156" s="4" t="s">
-        <v>633</v>
       </c>
       <c r="F156" s="4" t="s">
         <v>20</v>
@@ -11099,7 +11093,7 @@
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
       <c r="R156" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="S156" s="17">
         <v>42196</v>
@@ -11110,19 +11104,19 @@
     </row>
     <row r="157" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B157" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="E157" s="4" t="s">
         <v>635</v>
-      </c>
-      <c r="C157" s="6" t="s">
-        <v>774</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>636</v>
-      </c>
-      <c r="E157" s="4" t="s">
-        <v>637</v>
       </c>
       <c r="F157" s="4" t="s">
         <v>20</v>
@@ -11141,7 +11135,7 @@
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
       <c r="R157" s="4" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="S157" s="17">
         <v>42196</v>
@@ -11152,19 +11146,19 @@
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F158" s="4" t="s">
         <v>20</v>
@@ -11183,7 +11177,7 @@
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
       <c r="R158" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="S158" s="17">
         <v>42196</v>
@@ -11194,19 +11188,19 @@
     </row>
     <row r="159" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F159" s="4" t="s">
         <v>20</v>
@@ -11225,7 +11219,7 @@
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
       <c r="R159" s="4" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="S159" s="17">
         <v>42196</v>
@@ -11236,19 +11230,19 @@
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F160" s="4" t="s">
         <v>20</v>
@@ -11267,7 +11261,7 @@
       <c r="P160" s="4"/>
       <c r="Q160" s="4"/>
       <c r="R160" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="S160" s="17">
         <v>42196</v>
@@ -11278,19 +11272,19 @@
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="F161" s="4" t="s">
         <v>20</v>
@@ -11309,7 +11303,7 @@
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
       <c r="R161" s="4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="S161" s="17">
         <v>42196</v>
@@ -11320,19 +11314,19 @@
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F162" s="4" t="s">
         <v>20</v>
@@ -11351,7 +11345,7 @@
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
       <c r="R162" s="4" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="S162" s="17">
         <v>42196</v>
@@ -11362,19 +11356,19 @@
     </row>
     <row r="163" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F163" s="4" t="s">
         <v>20</v>
@@ -11393,7 +11387,7 @@
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
       <c r="R163" s="4" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="S163" s="17">
         <v>42196</v>
@@ -11404,19 +11398,19 @@
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F164" s="4" t="s">
         <v>20</v>
@@ -11435,7 +11429,7 @@
       <c r="P164" s="4"/>
       <c r="Q164" s="4"/>
       <c r="R164" s="4" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="S164" s="17">
         <v>42196</v>
@@ -11446,19 +11440,19 @@
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F165" s="4" t="s">
         <v>20</v>
@@ -11477,7 +11471,7 @@
       <c r="P165" s="4"/>
       <c r="Q165" s="4"/>
       <c r="R165" s="4" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="S165" s="17">
         <v>42196</v>
@@ -11488,19 +11482,19 @@
     </row>
     <row r="166" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B166" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D166" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="E166" s="4" t="s">
         <v>679</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D166" s="6" t="s">
-        <v>680</v>
-      </c>
-      <c r="E166" s="4" t="s">
-        <v>681</v>
       </c>
       <c r="F166" s="4" t="s">
         <v>20</v>
@@ -11519,7 +11513,7 @@
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
       <c r="R166" s="14" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="S166" s="17">
         <v>42196</v>
@@ -11530,19 +11524,19 @@
     </row>
     <row r="167" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B167" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>690</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D167" s="6" t="s">
-        <v>691</v>
-      </c>
-      <c r="E167" s="4" t="s">
-        <v>692</v>
       </c>
       <c r="F167" s="4" t="s">
         <v>20</v>
@@ -11561,7 +11555,7 @@
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
       <c r="R167" s="4" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="S167" s="17">
         <v>42196</v>
@@ -11572,19 +11566,19 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B168" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="E168" s="4" t="s">
         <v>711</v>
-      </c>
-      <c r="C168" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>712</v>
-      </c>
-      <c r="E168" s="4" t="s">
-        <v>713</v>
       </c>
       <c r="F168" s="4" t="s">
         <v>20</v>
@@ -11603,7 +11597,7 @@
       <c r="P168" s="4"/>
       <c r="Q168" s="4"/>
       <c r="R168" s="4" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="S168" s="17">
         <v>42196</v>
@@ -11614,25 +11608,25 @@
     </row>
     <row r="169" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B169" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D169" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="E169" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="C169" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D169" s="6" t="s">
+      <c r="F169" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G169" s="4" t="s">
         <v>716</v>
-      </c>
-      <c r="E169" s="4" t="s">
-        <v>717</v>
-      </c>
-      <c r="F169" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G169" s="4" t="s">
-        <v>718</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -11647,7 +11641,7 @@
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
       <c r="R169" s="4" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="S169" s="17">
         <v>42196</v>
@@ -11658,19 +11652,19 @@
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D170" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="E170" s="4" t="s">
         <v>720</v>
-      </c>
-      <c r="E170" s="4" t="s">
-        <v>722</v>
       </c>
       <c r="F170" s="4" t="s">
         <v>20</v>
@@ -11689,7 +11683,7 @@
       <c r="P170" s="4"/>
       <c r="Q170" s="4"/>
       <c r="R170" s="4" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="S170" s="17">
         <v>42196</v>
@@ -11700,19 +11694,19 @@
     </row>
     <row r="171" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B171" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D171" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="E171" s="4" t="s">
         <v>724</v>
-      </c>
-      <c r="C171" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D171" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="E171" s="4" t="s">
-        <v>726</v>
       </c>
       <c r="F171" s="4" t="s">
         <v>20</v>
@@ -11731,7 +11725,7 @@
       <c r="P171" s="4"/>
       <c r="Q171" s="4"/>
       <c r="R171" s="4" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="S171" s="17">
         <v>42196</v>
@@ -11742,29 +11736,29 @@
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B172" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="D172" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="C172" s="6" t="s">
-        <v>775</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>730</v>
-      </c>
       <c r="E172" s="4" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F172" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G172" s="4"/>
       <c r="H172" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I172" s="4" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J172" s="4"/>
       <c r="K172" s="4" t="s">
@@ -11777,7 +11771,7 @@
       <c r="P172" s="4"/>
       <c r="Q172" s="4"/>
       <c r="R172" s="4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="S172" s="17">
         <v>42196</v>
@@ -11788,19 +11782,19 @@
     </row>
     <row r="173" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B173" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D173" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="E173" s="4" t="s">
         <v>733</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D173" s="6" t="s">
-        <v>734</v>
-      </c>
-      <c r="E173" s="4" t="s">
-        <v>735</v>
       </c>
       <c r="F173" s="4" t="s">
         <v>20</v>
@@ -11819,7 +11813,7 @@
       <c r="P173" s="4"/>
       <c r="Q173" s="4"/>
       <c r="R173" s="4" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="S173" s="17">
         <v>42196</v>
@@ -11830,19 +11824,19 @@
     </row>
     <row r="174" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B174" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="E174" s="4" t="s">
         <v>737</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="D174" s="6" t="s">
-        <v>738</v>
-      </c>
-      <c r="E174" s="4" t="s">
-        <v>739</v>
       </c>
       <c r="F174" s="4" t="s">
         <v>20</v>
@@ -11861,7 +11855,7 @@
       <c r="P174" s="4"/>
       <c r="Q174" s="4"/>
       <c r="R174" s="4" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="S174" s="17">
         <v>42196</v>
@@ -11987,8 +11981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12012,10 +12006,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
@@ -12029,13 +12023,13 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>504</v>
+        <v>770</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="E2" s="18">
         <v>42196</v>
@@ -12044,7 +12038,7 @@
         <v>42196</v>
       </c>
       <c r="G2" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -12052,13 +12046,13 @@
         <v>90</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>504</v>
+        <v>770</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E3" s="18">
         <v>42196</v>
@@ -12067,7 +12061,7 @@
         <v>42196</v>
       </c>
       <c r="G3" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -12075,13 +12069,13 @@
         <v>125</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>540</v>
+        <v>771</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="E4" s="18">
         <v>42196</v>
@@ -12090,7 +12084,7 @@
         <v>42196</v>
       </c>
       <c r="G4" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -12098,13 +12092,13 @@
         <v>264</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>504</v>
+        <v>770</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="E5" s="18">
         <v>42196</v>
@@ -12113,7 +12107,7 @@
         <v>42196</v>
       </c>
       <c r="G5" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12121,13 +12115,13 @@
         <v>315</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>504</v>
+        <v>770</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="E6" s="18">
         <v>42196</v>
@@ -12136,22 +12130,22 @@
         <v>42196</v>
       </c>
       <c r="G6" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>759</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>754</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>762</v>
-      </c>
       <c r="E7" s="18">
         <v>42196</v>
       </c>
@@ -12159,7 +12153,7 @@
         <v>42196</v>
       </c>
       <c r="G7" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -12167,13 +12161,13 @@
         <v>388</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>758</v>
+        <v>801</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="E8" s="18">
         <v>42196</v>
@@ -12182,7 +12176,7 @@
         <v>42196</v>
       </c>
       <c r="G8" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12190,36 +12184,36 @@
         <v>413</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>758</v>
+        <v>801</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>766</v>
+      </c>
+      <c r="E9" s="18">
+        <v>42196</v>
+      </c>
+      <c r="F9" s="18">
+        <v>42196</v>
+      </c>
+      <c r="G9" t="s">
         <v>769</v>
-      </c>
-      <c r="E9" s="18">
-        <v>42196</v>
-      </c>
-      <c r="F9" s="18">
-        <v>42196</v>
-      </c>
-      <c r="G9" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>758</v>
+        <v>801</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="E10" s="18">
         <v>42196</v>
@@ -12228,7 +12222,7 @@
         <v>42196</v>
       </c>
       <c r="G10" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
   </sheetData>
@@ -12239,8 +12233,12 @@
     <hyperlink ref="B8" r:id="rId4"/>
     <hyperlink ref="B9" r:id="rId5"/>
     <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B3" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="B7" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>